<commit_message>
Fixed bug in Logger
</commit_message>
<xml_diff>
--- a/Code/output.xlsx
+++ b/Code/output.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -532,12 +532,353 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>75</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>80</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>85</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>90</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>95</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>100</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>105</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>110</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>115</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>120</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>125</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>130</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>135</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>140</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>145</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>150</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>155</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>160</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>165</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>170</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>175</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>180</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>185</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>190</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>195</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
         <v>200</v>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -552,7 +893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,7 +920,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -590,7 +931,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -601,7 +942,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -612,7 +953,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -623,7 +964,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -634,7 +975,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -645,7 +986,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -656,7 +997,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -667,12 +1008,353 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>75</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>80</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>85</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>90</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>95</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>100</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>105</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>110</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>115</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>120</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>125</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>130</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>135</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>140</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>145</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>150</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>155</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>160</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>165</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>170</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>175</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>180</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>185</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>190</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>195</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
         <v>200</v>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -687,7 +1369,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -714,101 +1396,442 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C3" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C4" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C5" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C6" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C7" t="n">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="B8" t="n">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="C8" t="n">
-        <v>52</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="B9" t="n">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="C9" t="n">
-        <v>39</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>117</v>
+      </c>
+      <c r="C10" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>125</v>
+      </c>
+      <c r="C11" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" t="n">
+        <v>133</v>
+      </c>
+      <c r="C12" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="n">
+        <v>143</v>
+      </c>
+      <c r="C13" t="n">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" t="n">
+        <v>154</v>
+      </c>
+      <c r="C14" t="n">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" t="n">
+        <v>165</v>
+      </c>
+      <c r="C15" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>75</v>
+      </c>
+      <c r="B16" t="n">
+        <v>174</v>
+      </c>
+      <c r="C16" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>80</v>
+      </c>
+      <c r="B17" t="n">
+        <v>184</v>
+      </c>
+      <c r="C17" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>85</v>
+      </c>
+      <c r="B18" t="n">
         <v>200</v>
       </c>
-      <c r="B10" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" t="n">
-        <v>3</v>
+      <c r="C18" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>90</v>
+      </c>
+      <c r="B19" t="n">
+        <v>210</v>
+      </c>
+      <c r="C19" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>95</v>
+      </c>
+      <c r="B20" t="n">
+        <v>216</v>
+      </c>
+      <c r="C20" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>100</v>
+      </c>
+      <c r="B21" t="n">
+        <v>225</v>
+      </c>
+      <c r="C21" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>105</v>
+      </c>
+      <c r="B22" t="n">
+        <v>237</v>
+      </c>
+      <c r="C22" t="n">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>110</v>
+      </c>
+      <c r="B23" t="n">
+        <v>248</v>
+      </c>
+      <c r="C23" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>115</v>
+      </c>
+      <c r="B24" t="n">
+        <v>258</v>
+      </c>
+      <c r="C24" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>120</v>
+      </c>
+      <c r="B25" t="n">
+        <v>270</v>
+      </c>
+      <c r="C25" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>125</v>
+      </c>
+      <c r="B26" t="n">
+        <v>280</v>
+      </c>
+      <c r="C26" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>130</v>
+      </c>
+      <c r="B27" t="n">
+        <v>288</v>
+      </c>
+      <c r="C27" t="n">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>135</v>
+      </c>
+      <c r="B28" t="n">
+        <v>295</v>
+      </c>
+      <c r="C28" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>140</v>
+      </c>
+      <c r="B29" t="n">
+        <v>303</v>
+      </c>
+      <c r="C29" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>145</v>
+      </c>
+      <c r="B30" t="n">
+        <v>312</v>
+      </c>
+      <c r="C30" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>150</v>
+      </c>
+      <c r="B31" t="n">
+        <v>318</v>
+      </c>
+      <c r="C31" t="n">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>155</v>
+      </c>
+      <c r="B32" t="n">
+        <v>322</v>
+      </c>
+      <c r="C32" t="n">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>160</v>
+      </c>
+      <c r="B33" t="n">
+        <v>330</v>
+      </c>
+      <c r="C33" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>165</v>
+      </c>
+      <c r="B34" t="n">
+        <v>341</v>
+      </c>
+      <c r="C34" t="n">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>170</v>
+      </c>
+      <c r="B35" t="n">
+        <v>349</v>
+      </c>
+      <c r="C35" t="n">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>175</v>
+      </c>
+      <c r="B36" t="n">
+        <v>358</v>
+      </c>
+      <c r="C36" t="n">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>180</v>
+      </c>
+      <c r="B37" t="n">
+        <v>368</v>
+      </c>
+      <c r="C37" t="n">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>185</v>
+      </c>
+      <c r="B38" t="n">
+        <v>377</v>
+      </c>
+      <c r="C38" t="n">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>190</v>
+      </c>
+      <c r="B39" t="n">
+        <v>385</v>
+      </c>
+      <c r="C39" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>195</v>
+      </c>
+      <c r="B40" t="n">
+        <v>392</v>
+      </c>
+      <c r="C40" t="n">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>200</v>
+      </c>
+      <c r="B41" t="n">
+        <v>396</v>
+      </c>
+      <c r="C41" t="n">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +1845,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -854,7 +1877,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -863,12 +1886,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -877,12 +1900,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -891,12 +1914,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -905,12 +1928,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -919,12 +1942,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -933,12 +1956,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -947,12 +1970,12 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>52</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -961,21 +1984,455 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>39</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>75</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>80</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>85</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
         <v>200</v>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3</v>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>90</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>95</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>100</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>105</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>110</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>115</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>120</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>125</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>130</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>135</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>140</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>145</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>150</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>155</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>160</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>165</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>170</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>175</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>180</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>185</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>190</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>195</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>200</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +2446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1021,7 +2478,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -1030,12 +2487,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -1044,12 +2501,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -1058,12 +2515,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -1072,12 +2529,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -1086,12 +2543,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1100,12 +2557,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -1114,12 +2571,12 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>52</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -1128,21 +2585,455 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>39</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>75</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>80</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>85</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
         <v>200</v>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3</v>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>90</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>95</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>100</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>105</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>110</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>115</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>120</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>125</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>130</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>135</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>140</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>145</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>150</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>155</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>160</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>165</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>170</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>175</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>180</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>185</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>190</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>195</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>200</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preferential queue and preferential queue tests
</commit_message>
<xml_diff>
--- a/Code/output.xlsx
+++ b/Code/output.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -882,6 +882,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>205</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -893,7 +904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1358,6 +1369,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>205</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1369,7 +1391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1399,10 +1421,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -1410,10 +1432,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -1421,10 +1443,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -1432,10 +1454,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
@@ -1443,10 +1465,10 @@
         <v>25</v>
       </c>
       <c r="B6" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -1454,10 +1476,10 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
@@ -1465,10 +1487,10 @@
         <v>35</v>
       </c>
       <c r="B8" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C8" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
@@ -1476,10 +1498,10 @@
         <v>40</v>
       </c>
       <c r="B9" t="n">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C9" t="n">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10">
@@ -1487,10 +1509,10 @@
         <v>45</v>
       </c>
       <c r="B10" t="n">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C10" t="n">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11">
@@ -1498,10 +1520,10 @@
         <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C11" t="n">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12">
@@ -1509,10 +1531,10 @@
         <v>55</v>
       </c>
       <c r="B12" t="n">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C12" t="n">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13">
@@ -1520,10 +1542,10 @@
         <v>60</v>
       </c>
       <c r="B13" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C13" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14">
@@ -1531,10 +1553,10 @@
         <v>65</v>
       </c>
       <c r="B14" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C14" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15">
@@ -1542,10 +1564,10 @@
         <v>70</v>
       </c>
       <c r="B15" t="n">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C15" t="n">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
@@ -1553,10 +1575,10 @@
         <v>75</v>
       </c>
       <c r="B16" t="n">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C16" t="n">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17">
@@ -1564,10 +1586,10 @@
         <v>80</v>
       </c>
       <c r="B17" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C17" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18">
@@ -1575,10 +1597,10 @@
         <v>85</v>
       </c>
       <c r="B18" t="n">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C18" t="n">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19">
@@ -1586,10 +1608,10 @@
         <v>90</v>
       </c>
       <c r="B19" t="n">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C19" t="n">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20">
@@ -1597,10 +1619,10 @@
         <v>95</v>
       </c>
       <c r="B20" t="n">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C20" t="n">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21">
@@ -1608,10 +1630,10 @@
         <v>100</v>
       </c>
       <c r="B21" t="n">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C21" t="n">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22">
@@ -1619,10 +1641,10 @@
         <v>105</v>
       </c>
       <c r="B22" t="n">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="C22" t="n">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23">
@@ -1630,10 +1652,10 @@
         <v>110</v>
       </c>
       <c r="B23" t="n">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C23" t="n">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24">
@@ -1641,10 +1663,10 @@
         <v>115</v>
       </c>
       <c r="B24" t="n">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C24" t="n">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
@@ -1652,10 +1674,10 @@
         <v>120</v>
       </c>
       <c r="B25" t="n">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="C25" t="n">
-        <v>270</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26">
@@ -1663,10 +1685,10 @@
         <v>125</v>
       </c>
       <c r="B26" t="n">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="C26" t="n">
-        <v>280</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27">
@@ -1674,10 +1696,10 @@
         <v>130</v>
       </c>
       <c r="B27" t="n">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="C27" t="n">
-        <v>288</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28">
@@ -1685,10 +1707,10 @@
         <v>135</v>
       </c>
       <c r="B28" t="n">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="C28" t="n">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29">
@@ -1696,10 +1718,10 @@
         <v>140</v>
       </c>
       <c r="B29" t="n">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="C29" t="n">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30">
@@ -1707,10 +1729,10 @@
         <v>145</v>
       </c>
       <c r="B30" t="n">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="C30" t="n">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31">
@@ -1718,10 +1740,10 @@
         <v>150</v>
       </c>
       <c r="B31" t="n">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C31" t="n">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32">
@@ -1729,10 +1751,10 @@
         <v>155</v>
       </c>
       <c r="B32" t="n">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C32" t="n">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33">
@@ -1740,10 +1762,10 @@
         <v>160</v>
       </c>
       <c r="B33" t="n">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C33" t="n">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="34">
@@ -1751,10 +1773,10 @@
         <v>165</v>
       </c>
       <c r="B34" t="n">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C34" t="n">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35">
@@ -1762,10 +1784,10 @@
         <v>170</v>
       </c>
       <c r="B35" t="n">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C35" t="n">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36">
@@ -1773,10 +1795,10 @@
         <v>175</v>
       </c>
       <c r="B36" t="n">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C36" t="n">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37">
@@ -1784,10 +1806,10 @@
         <v>180</v>
       </c>
       <c r="B37" t="n">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C37" t="n">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="38">
@@ -1795,10 +1817,10 @@
         <v>185</v>
       </c>
       <c r="B38" t="n">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C38" t="n">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39">
@@ -1806,10 +1828,10 @@
         <v>190</v>
       </c>
       <c r="B39" t="n">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C39" t="n">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="40">
@@ -1817,10 +1839,10 @@
         <v>195</v>
       </c>
       <c r="B40" t="n">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C40" t="n">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="41">
@@ -1828,9 +1850,20 @@
         <v>200</v>
       </c>
       <c r="B41" t="n">
+        <v>395</v>
+      </c>
+      <c r="C41" t="n">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>205</v>
+      </c>
+      <c r="B42" t="n">
         <v>396</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C42" t="n">
         <v>396</v>
       </c>
     </row>
@@ -1845,7 +1878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1886,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -1900,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -1914,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -1928,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
@@ -1942,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -1956,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
@@ -1970,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
@@ -1984,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10">
@@ -1998,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11">
@@ -2012,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12">
@@ -2026,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13">
@@ -2040,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14">
@@ -2054,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15">
@@ -2068,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
@@ -2082,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17">
@@ -2096,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18">
@@ -2110,7 +2143,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19">
@@ -2124,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20">
@@ -2138,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21">
@@ -2152,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22">
@@ -2166,7 +2199,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23">
@@ -2180,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24">
@@ -2194,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
@@ -2208,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>270</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26">
@@ -2222,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>280</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27">
@@ -2236,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>288</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28">
@@ -2250,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29">
@@ -2264,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30">
@@ -2278,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31">
@@ -2292,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32">
@@ -2306,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33">
@@ -2320,7 +2353,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="34">
@@ -2334,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35">
@@ -2348,7 +2381,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36">
@@ -2362,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37">
@@ -2376,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="38">
@@ -2390,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39">
@@ -2404,7 +2437,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="40">
@@ -2418,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="41">
@@ -2432,6 +2465,20 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>205</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
         <v>396</v>
       </c>
     </row>
@@ -2446,7 +2493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2487,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -2501,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -2515,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -2529,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
@@ -2543,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -2557,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
@@ -2571,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
@@ -2585,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10">
@@ -2599,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11">
@@ -2613,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12">
@@ -2627,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13">
@@ -2641,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14">
@@ -2655,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15">
@@ -2669,7 +2716,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
@@ -2683,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17">
@@ -2697,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18">
@@ -2711,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19">
@@ -2725,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20">
@@ -2739,7 +2786,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21">
@@ -2753,7 +2800,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22">
@@ -2767,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23">
@@ -2781,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24">
@@ -2795,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
@@ -2809,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>270</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26">
@@ -2823,7 +2870,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>280</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27">
@@ -2837,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>288</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28">
@@ -2851,7 +2898,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29">
@@ -2865,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30">
@@ -2879,7 +2926,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31">
@@ -2893,7 +2940,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32">
@@ -2907,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33">
@@ -2921,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="34">
@@ -2935,7 +2982,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35">
@@ -2949,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36">
@@ -2963,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37">
@@ -2977,7 +3024,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="38">
@@ -2991,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39">
@@ -3005,7 +3052,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="40">
@@ -3019,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="41">
@@ -3033,6 +3080,20 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>205</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
         <v>396</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented force param in queue.push_request()
</commit_message>
<xml_diff>
--- a/Code/output.xlsx
+++ b/Code/output.xlsx
@@ -10,8 +10,8 @@
     <sheet name="success" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="fail" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="network" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="0TestDistributor" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="1TestDistributor" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="0OriginalSequentialForwarding" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="1OriginalSequentialForwarding" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,12 +433,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>0TestDistributor</t>
+          <t>0OriginalSequentialForwarding</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>1TestDistributor</t>
+          <t>1OriginalSequentialForwarding</t>
         </is>
       </c>
     </row>
@@ -890,6 +890,28 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>210</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>215</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -904,7 +926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -920,12 +942,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>0TestDistributor</t>
+          <t>0OriginalSequentialForwarding</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>1TestDistributor</t>
+          <t>1OriginalSequentialForwarding</t>
         </is>
       </c>
     </row>
@@ -1377,6 +1399,28 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>210</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>215</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1391,7 +1435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1407,12 +1451,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>0TestDistributor</t>
+          <t>0OriginalSequentialForwarding</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>1TestDistributor</t>
+          <t>1OriginalSequentialForwarding</t>
         </is>
       </c>
     </row>
@@ -1421,10 +1465,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -1432,10 +1476,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -1443,10 +1487,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C4" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -1454,10 +1498,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C5" t="n">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
@@ -1465,10 +1509,10 @@
         <v>25</v>
       </c>
       <c r="B6" t="n">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C6" t="n">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
@@ -1476,10 +1520,10 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C7" t="n">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
@@ -1487,10 +1531,10 @@
         <v>35</v>
       </c>
       <c r="B8" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C8" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9">
@@ -1498,10 +1542,10 @@
         <v>40</v>
       </c>
       <c r="B9" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="C9" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10">
@@ -1509,10 +1553,10 @@
         <v>45</v>
       </c>
       <c r="B10" t="n">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="C10" t="n">
-        <v>121</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11">
@@ -1520,10 +1564,10 @@
         <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="C11" t="n">
-        <v>131</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12">
@@ -1531,10 +1575,10 @@
         <v>55</v>
       </c>
       <c r="B12" t="n">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="C12" t="n">
-        <v>141</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13">
@@ -1542,10 +1586,10 @@
         <v>60</v>
       </c>
       <c r="B13" t="n">
-        <v>146</v>
+        <v>210</v>
       </c>
       <c r="C13" t="n">
-        <v>146</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14">
@@ -1553,10 +1597,10 @@
         <v>65</v>
       </c>
       <c r="B14" t="n">
-        <v>155</v>
+        <v>228</v>
       </c>
       <c r="C14" t="n">
-        <v>155</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15">
@@ -1564,10 +1608,10 @@
         <v>70</v>
       </c>
       <c r="B15" t="n">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="C15" t="n">
-        <v>170</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16">
@@ -1575,10 +1619,10 @@
         <v>75</v>
       </c>
       <c r="B16" t="n">
-        <v>180</v>
+        <v>260</v>
       </c>
       <c r="C16" t="n">
-        <v>180</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17">
@@ -1586,10 +1630,10 @@
         <v>80</v>
       </c>
       <c r="B17" t="n">
-        <v>185</v>
+        <v>280</v>
       </c>
       <c r="C17" t="n">
-        <v>185</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18">
@@ -1597,10 +1641,10 @@
         <v>85</v>
       </c>
       <c r="B18" t="n">
-        <v>191</v>
+        <v>303</v>
       </c>
       <c r="C18" t="n">
-        <v>191</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19">
@@ -1608,10 +1652,10 @@
         <v>90</v>
       </c>
       <c r="B19" t="n">
-        <v>199</v>
+        <v>328</v>
       </c>
       <c r="C19" t="n">
-        <v>199</v>
+        <v>328</v>
       </c>
     </row>
     <row r="20">
@@ -1619,10 +1663,10 @@
         <v>95</v>
       </c>
       <c r="B20" t="n">
-        <v>206</v>
+        <v>354</v>
       </c>
       <c r="C20" t="n">
-        <v>206</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21">
@@ -1630,10 +1674,10 @@
         <v>100</v>
       </c>
       <c r="B21" t="n">
-        <v>214</v>
+        <v>378</v>
       </c>
       <c r="C21" t="n">
-        <v>214</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22">
@@ -1641,10 +1685,10 @@
         <v>105</v>
       </c>
       <c r="B22" t="n">
-        <v>224</v>
+        <v>402</v>
       </c>
       <c r="C22" t="n">
-        <v>224</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23">
@@ -1652,10 +1696,10 @@
         <v>110</v>
       </c>
       <c r="B23" t="n">
-        <v>236</v>
+        <v>423</v>
       </c>
       <c r="C23" t="n">
-        <v>236</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24">
@@ -1663,10 +1707,10 @@
         <v>115</v>
       </c>
       <c r="B24" t="n">
-        <v>249</v>
+        <v>446</v>
       </c>
       <c r="C24" t="n">
-        <v>249</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25">
@@ -1674,10 +1718,10 @@
         <v>120</v>
       </c>
       <c r="B25" t="n">
-        <v>257</v>
+        <v>466</v>
       </c>
       <c r="C25" t="n">
-        <v>257</v>
+        <v>466</v>
       </c>
     </row>
     <row r="26">
@@ -1685,10 +1729,10 @@
         <v>125</v>
       </c>
       <c r="B26" t="n">
-        <v>261</v>
+        <v>486</v>
       </c>
       <c r="C26" t="n">
-        <v>261</v>
+        <v>486</v>
       </c>
     </row>
     <row r="27">
@@ -1696,10 +1740,10 @@
         <v>130</v>
       </c>
       <c r="B27" t="n">
-        <v>264</v>
+        <v>509</v>
       </c>
       <c r="C27" t="n">
-        <v>264</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28">
@@ -1707,10 +1751,10 @@
         <v>135</v>
       </c>
       <c r="B28" t="n">
-        <v>275</v>
+        <v>533</v>
       </c>
       <c r="C28" t="n">
-        <v>275</v>
+        <v>533</v>
       </c>
     </row>
     <row r="29">
@@ -1718,10 +1762,10 @@
         <v>140</v>
       </c>
       <c r="B29" t="n">
-        <v>289</v>
+        <v>556</v>
       </c>
       <c r="C29" t="n">
-        <v>289</v>
+        <v>556</v>
       </c>
     </row>
     <row r="30">
@@ -1729,10 +1773,10 @@
         <v>145</v>
       </c>
       <c r="B30" t="n">
-        <v>300</v>
+        <v>575</v>
       </c>
       <c r="C30" t="n">
-        <v>300</v>
+        <v>575</v>
       </c>
     </row>
     <row r="31">
@@ -1740,10 +1784,10 @@
         <v>150</v>
       </c>
       <c r="B31" t="n">
-        <v>310</v>
+        <v>594</v>
       </c>
       <c r="C31" t="n">
-        <v>310</v>
+        <v>594</v>
       </c>
     </row>
     <row r="32">
@@ -1751,10 +1795,10 @@
         <v>155</v>
       </c>
       <c r="B32" t="n">
-        <v>318</v>
+        <v>612</v>
       </c>
       <c r="C32" t="n">
-        <v>318</v>
+        <v>612</v>
       </c>
     </row>
     <row r="33">
@@ -1762,10 +1806,10 @@
         <v>160</v>
       </c>
       <c r="B33" t="n">
-        <v>325</v>
+        <v>627</v>
       </c>
       <c r="C33" t="n">
-        <v>325</v>
+        <v>627</v>
       </c>
     </row>
     <row r="34">
@@ -1773,10 +1817,10 @@
         <v>165</v>
       </c>
       <c r="B34" t="n">
-        <v>335</v>
+        <v>645</v>
       </c>
       <c r="C34" t="n">
-        <v>335</v>
+        <v>645</v>
       </c>
     </row>
     <row r="35">
@@ -1784,10 +1828,10 @@
         <v>170</v>
       </c>
       <c r="B35" t="n">
-        <v>346</v>
+        <v>659</v>
       </c>
       <c r="C35" t="n">
-        <v>346</v>
+        <v>659</v>
       </c>
     </row>
     <row r="36">
@@ -1795,10 +1839,10 @@
         <v>175</v>
       </c>
       <c r="B36" t="n">
-        <v>355</v>
+        <v>668</v>
       </c>
       <c r="C36" t="n">
-        <v>355</v>
+        <v>668</v>
       </c>
     </row>
     <row r="37">
@@ -1806,10 +1850,10 @@
         <v>180</v>
       </c>
       <c r="B37" t="n">
-        <v>363</v>
+        <v>683</v>
       </c>
       <c r="C37" t="n">
-        <v>363</v>
+        <v>683</v>
       </c>
     </row>
     <row r="38">
@@ -1817,10 +1861,10 @@
         <v>185</v>
       </c>
       <c r="B38" t="n">
-        <v>371</v>
+        <v>702</v>
       </c>
       <c r="C38" t="n">
-        <v>371</v>
+        <v>702</v>
       </c>
     </row>
     <row r="39">
@@ -1828,10 +1872,10 @@
         <v>190</v>
       </c>
       <c r="B39" t="n">
-        <v>379</v>
+        <v>722</v>
       </c>
       <c r="C39" t="n">
-        <v>379</v>
+        <v>722</v>
       </c>
     </row>
     <row r="40">
@@ -1839,10 +1883,10 @@
         <v>195</v>
       </c>
       <c r="B40" t="n">
-        <v>388</v>
+        <v>747</v>
       </c>
       <c r="C40" t="n">
-        <v>388</v>
+        <v>747</v>
       </c>
     </row>
     <row r="41">
@@ -1850,10 +1894,10 @@
         <v>200</v>
       </c>
       <c r="B41" t="n">
-        <v>395</v>
+        <v>768</v>
       </c>
       <c r="C41" t="n">
-        <v>395</v>
+        <v>768</v>
       </c>
     </row>
     <row r="42">
@@ -1861,10 +1905,32 @@
         <v>205</v>
       </c>
       <c r="B42" t="n">
-        <v>396</v>
+        <v>780</v>
       </c>
       <c r="C42" t="n">
-        <v>396</v>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>210</v>
+      </c>
+      <c r="B43" t="n">
+        <v>789</v>
+      </c>
+      <c r="C43" t="n">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>215</v>
+      </c>
+      <c r="B44" t="n">
+        <v>792</v>
+      </c>
+      <c r="C44" t="n">
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -1878,7 +1944,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1919,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -1933,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -1947,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -1961,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
@@ -1975,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
@@ -1989,7 +2055,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
@@ -2003,7 +2069,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9">
@@ -2017,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10">
@@ -2031,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>121</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11">
@@ -2045,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>131</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12">
@@ -2059,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>141</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13">
@@ -2073,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>146</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14">
@@ -2087,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>155</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15">
@@ -2101,7 +2167,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>170</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16">
@@ -2115,7 +2181,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>180</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17">
@@ -2129,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>185</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18">
@@ -2143,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>191</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19">
@@ -2157,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>199</v>
+        <v>328</v>
       </c>
     </row>
     <row r="20">
@@ -2171,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>206</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21">
@@ -2185,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>214</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22">
@@ -2199,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>224</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23">
@@ -2213,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>236</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24">
@@ -2227,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>249</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25">
@@ -2241,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>257</v>
+        <v>466</v>
       </c>
     </row>
     <row r="26">
@@ -2255,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>261</v>
+        <v>486</v>
       </c>
     </row>
     <row r="27">
@@ -2269,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>264</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28">
@@ -2283,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>275</v>
+        <v>533</v>
       </c>
     </row>
     <row r="29">
@@ -2297,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>289</v>
+        <v>556</v>
       </c>
     </row>
     <row r="30">
@@ -2311,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>300</v>
+        <v>575</v>
       </c>
     </row>
     <row r="31">
@@ -2325,7 +2391,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>310</v>
+        <v>594</v>
       </c>
     </row>
     <row r="32">
@@ -2339,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>318</v>
+        <v>612</v>
       </c>
     </row>
     <row r="33">
@@ -2353,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>325</v>
+        <v>627</v>
       </c>
     </row>
     <row r="34">
@@ -2367,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>335</v>
+        <v>645</v>
       </c>
     </row>
     <row r="35">
@@ -2381,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>346</v>
+        <v>659</v>
       </c>
     </row>
     <row r="36">
@@ -2395,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>355</v>
+        <v>668</v>
       </c>
     </row>
     <row r="37">
@@ -2409,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>363</v>
+        <v>683</v>
       </c>
     </row>
     <row r="38">
@@ -2423,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>371</v>
+        <v>702</v>
       </c>
     </row>
     <row r="39">
@@ -2437,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>379</v>
+        <v>722</v>
       </c>
     </row>
     <row r="40">
@@ -2451,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>388</v>
+        <v>747</v>
       </c>
     </row>
     <row r="41">
@@ -2465,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>395</v>
+        <v>768</v>
       </c>
     </row>
     <row r="42">
@@ -2479,7 +2545,35 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>396</v>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>210</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>215</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -2493,7 +2587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2534,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -2548,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -2562,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -2576,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
@@ -2590,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
@@ -2604,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
@@ -2618,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9">
@@ -2632,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10">
@@ -2646,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>121</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11">
@@ -2660,7 +2754,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>131</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12">
@@ -2674,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>141</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13">
@@ -2688,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>146</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14">
@@ -2702,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>155</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15">
@@ -2716,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>170</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16">
@@ -2730,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>180</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17">
@@ -2744,7 +2838,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>185</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18">
@@ -2758,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>191</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19">
@@ -2772,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>199</v>
+        <v>328</v>
       </c>
     </row>
     <row r="20">
@@ -2786,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>206</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21">
@@ -2800,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>214</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22">
@@ -2814,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>224</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23">
@@ -2828,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>236</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24">
@@ -2842,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>249</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25">
@@ -2856,7 +2950,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>257</v>
+        <v>466</v>
       </c>
     </row>
     <row r="26">
@@ -2870,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>261</v>
+        <v>486</v>
       </c>
     </row>
     <row r="27">
@@ -2884,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>264</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28">
@@ -2898,7 +2992,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>275</v>
+        <v>533</v>
       </c>
     </row>
     <row r="29">
@@ -2912,7 +3006,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>289</v>
+        <v>556</v>
       </c>
     </row>
     <row r="30">
@@ -2926,7 +3020,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>300</v>
+        <v>575</v>
       </c>
     </row>
     <row r="31">
@@ -2940,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>310</v>
+        <v>594</v>
       </c>
     </row>
     <row r="32">
@@ -2954,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>318</v>
+        <v>612</v>
       </c>
     </row>
     <row r="33">
@@ -2968,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>325</v>
+        <v>627</v>
       </c>
     </row>
     <row r="34">
@@ -2982,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>335</v>
+        <v>645</v>
       </c>
     </row>
     <row r="35">
@@ -2996,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>346</v>
+        <v>659</v>
       </c>
     </row>
     <row r="36">
@@ -3010,7 +3104,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>355</v>
+        <v>668</v>
       </c>
     </row>
     <row r="37">
@@ -3024,7 +3118,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>363</v>
+        <v>683</v>
       </c>
     </row>
     <row r="38">
@@ -3038,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>371</v>
+        <v>702</v>
       </c>
     </row>
     <row r="39">
@@ -3052,7 +3146,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>379</v>
+        <v>722</v>
       </c>
     </row>
     <row r="40">
@@ -3066,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>388</v>
+        <v>747</v>
       </c>
     </row>
     <row r="41">
@@ -3080,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>395</v>
+        <v>768</v>
       </c>
     </row>
     <row r="42">
@@ -3094,7 +3188,35 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>396</v>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>210</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>215</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>